<commit_message>
Production ready: Complete bill generation system with notesheet, extra items slip, and enterprise features
</commit_message>
<xml_diff>
--- a/TEST_INPUT_FILES/FirstFINALvidExtra.xlsx
+++ b/TEST_INPUT_FILES/FirstFINALvidExtra.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajkumar\Documents\000 test_files\BILLS\new pattern\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajkumar\BillGeneratorUnified\TEST_INPUT_FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="615"/>
+    <workbookView minimized="1" xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="615"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="117">
   <si>
     <t>Item</t>
   </si>
@@ -387,9 +387,6 @@
   </si>
   <si>
     <t>M/s. Shree Krishna Builders Jaipur</t>
-  </si>
-  <si>
-    <t>First Final   First &amp; Final Bill Not Applicable 2145 Dt. 15-02-2025 72/2024-25 478510 15-02-25 22-02-25 10-05-25 19-07-25 07-04-25 3.75 Below 0</t>
   </si>
   <si>
     <t>Plumbing Installation and MTC work at Govt. Nehru hostel Mansarovar, Sanganer, Jaipur</t>
@@ -1053,10 +1050,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1066,12 +1063,12 @@
     <col min="3" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="32" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:2" s="32" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="32" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:2" s="32" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="40" t="s">
         <v>105</v>
       </c>
@@ -1079,7 +1076,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="32" customFormat="1" ht="15" customHeight="1">
+    <row r="3" spans="1:2" s="32" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="40" t="s">
         <v>107</v>
       </c>
@@ -1087,16 +1084,13 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="32" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:2" s="32" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="40" t="s">
         <v>109</v>
       </c>
       <c r="B4" s="40"/>
-      <c r="D4" s="32" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="32" customFormat="1" ht="12">
+    </row>
+    <row r="5" spans="1:2" s="32" customFormat="1" ht="12">
       <c r="A5" s="33" t="s">
         <v>79</v>
       </c>
@@ -1104,15 +1098,15 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="32" customFormat="1" ht="12">
+    <row r="6" spans="1:2" s="32" customFormat="1" ht="12">
       <c r="A6" s="33" t="s">
         <v>80</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="32" customFormat="1" ht="12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="32" customFormat="1" ht="12">
       <c r="A7" s="33" t="s">
         <v>81</v>
       </c>
@@ -1120,7 +1114,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="32" customFormat="1" ht="12">
+    <row r="8" spans="1:2" s="32" customFormat="1" ht="12">
       <c r="A8" s="33" t="s">
         <v>82</v>
       </c>
@@ -1128,15 +1122,15 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="32" customFormat="1" ht="12">
+    <row r="9" spans="1:2" s="32" customFormat="1" ht="12">
       <c r="A9" s="33" t="s">
         <v>84</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="32" customFormat="1" ht="12">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="32" customFormat="1" ht="12">
       <c r="A10" s="33" t="s">
         <v>69</v>
       </c>
@@ -1144,7 +1138,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="11" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>112</v>
       </c>
@@ -1153,7 +1147,7 @@
         <v>355874</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="32" customFormat="1" ht="12">
+    <row r="12" spans="1:2" s="32" customFormat="1" ht="12">
       <c r="A12" s="33" t="s">
         <v>48</v>
       </c>
@@ -1161,7 +1155,7 @@
         <v>45601</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="32" customFormat="1" ht="15" customHeight="1">
+    <row r="13" spans="1:2" s="32" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="33" t="s">
         <v>73</v>
       </c>
@@ -1170,7 +1164,7 @@
         <v>45608</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="32" customFormat="1" ht="15" customHeight="1">
+    <row r="14" spans="1:2" s="32" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="33" t="s">
         <v>70</v>
       </c>
@@ -1179,7 +1173,7 @@
         <v>45878</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="32" customFormat="1" ht="12">
+    <row r="15" spans="1:2" s="32" customFormat="1" ht="12">
       <c r="A15" s="33" t="s">
         <v>71</v>
       </c>
@@ -1188,7 +1182,7 @@
         <v>45883</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="32" customFormat="1" ht="15" customHeight="1">
+    <row r="16" spans="1:2" s="32" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="33" t="s">
         <v>72</v>
       </c>
@@ -1234,7 +1228,7 @@
   </sheetPr>
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>

</xml_diff>